<commit_message>
Atualização automática de TAQUARA.xlsx
</commit_message>
<xml_diff>
--- a/TAQUARA.xlsx
+++ b/TAQUARA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFE23FC3-90DE-4DF5-ADF8-4C778FCC96E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5195BF3-2BAA-40B0-A35F-B40BDEB80DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1471,7 +1471,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{27688CB6-38CB-4724-A917-EAD3EC021BAA}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{76333346-4F3D-4156-819A-83A570C4073C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1501,10 +1501,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B2592B7-ECB3-4998-A92C-B498BE8F8C8F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{424EDD2C-9EDA-4EAC-85CF-883EC9A51D11}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1542,7 +1542,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2AE4A4-C8F8-4361-89B9-8F822BAD2A74}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F7FCB72-67BD-465B-87F3-C8EC44D6F8E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1605,7 +1605,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D0719D-4640-4FDB-BA79-0EA6A0962A5A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ADC400D-59DA-4E40-9747-922ED94E3A38}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1624,7 +1624,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE1B31B0-F172-12EB-8B35-16013D87718B}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA2E1D05-D115-1FDE-A316-D091A9369612}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1673,7 +1673,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD173C30-4411-72E6-7481-43B61D13DAE4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{100B27AE-B08B-045D-4FBC-A45172B60746}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1692,7 +1692,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5280C7B5-1EEA-2D92-893B-97A58B234280}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B8BEF27-541C-FE45-A58A-34E4FCEC927B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1723,7 +1723,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF980328-7641-B9F4-95C5-92796A490828}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65B45D27-F5C4-E24E-7349-B880BA5B3B37}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1754,7 +1754,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8299EE79-24F8-9C9F-E9B4-C98798561CF9}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5037F8A8-1B80-E8CF-BB92-8E08B5F078B1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1797,7 +1797,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F480BF-675A-4427-8C79-54B93101DC3E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2349DF09-36E0-4763-883E-5F06AB99D220}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1835,7 +1835,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD2B2FF4-16BE-4DF6-B02F-D379331BDE57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D59C4E5D-2F46-4C17-9764-55AE4ECE8BB1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1878,7 +1878,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70E528E3-A4D9-4A11-BBC0-B05CB1E52546}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDDA3C45-E94F-4AE1-87E0-E80302AB866D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2191,7 +2191,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F07D71-DAC1-4E11-912F-AC6CCD155235}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE0C46F-11CE-467F-A397-A365E6E3307B}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>